<commit_message>
updates to the readme file
</commit_message>
<xml_diff>
--- a/inst/extdata/example_figure_data.xlsx
+++ b/inst/extdata/example_figure_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Randy\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\forestable\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{457E4663-B538-44D4-B2FE-7EB8AF6C2E06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEC6D54-17EA-47D5-9562-E2142C27F087}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21684" yWindow="7656" windowWidth="28380" windowHeight="16368" xr2:uid="{97D096E3-90A8-4D25-ADEB-070196C0D950}"/>
+    <workbookView xWindow="5568" yWindow="1128" windowWidth="28380" windowHeight="14724" xr2:uid="{97D096E3-90A8-4D25-ADEB-070196C0D950}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,90 +51,27 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Female</t>
-  </si>
-  <si>
     <t>Age</t>
   </si>
   <si>
-    <t>&lt;65 yr</t>
-  </si>
-  <si>
-    <t>&lt;75 yr</t>
-  </si>
-  <si>
-    <t>&gt;65 yr</t>
-  </si>
-  <si>
-    <t>&gt;75 yr</t>
-  </si>
-  <si>
     <t>Body-mass index</t>
   </si>
   <si>
-    <t>&lt;Median</t>
-  </si>
-  <si>
-    <t>&gt;Median</t>
-  </si>
-  <si>
     <t>Race</t>
   </si>
   <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Baseline Statin Treatment</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>Intensity of statin treatment</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Not High</t>
-  </si>
-  <si>
     <t>Metabolic disease</t>
   </si>
   <si>
-    <t>Diabetes</t>
-  </si>
-  <si>
-    <t>Metabolic syndrome</t>
-  </si>
-  <si>
-    <t>Neither</t>
-  </si>
-  <si>
     <t>Renal function</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Mild Impairment</t>
-  </si>
-  <si>
-    <t>Moderate impairment</t>
-  </si>
-  <si>
     <t>Estimate</t>
   </si>
   <si>
@@ -142,6 +79,69 @@
   </si>
   <si>
     <t>CI high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;65 yr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &gt;65 yr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;75 yr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &gt;75 yr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;Median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &gt;Median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Black</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Not High</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Diabetes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Metabolic syndrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Neither</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Normal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Mild Impairment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Moderate impairment</t>
   </si>
 </sst>
 </file>
@@ -496,7 +496,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -515,13 +515,13 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -551,7 +551,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>535</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>246</v>
@@ -591,12 +591,12 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B7">
         <v>297</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>484</v>
@@ -636,7 +636,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>638</v>
@@ -656,7 +656,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B10">
         <v>143</v>
@@ -676,12 +676,12 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>394</v>
@@ -701,7 +701,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>387</v>
@@ -721,12 +721,12 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B15">
         <v>653</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B16">
         <v>110</v>
@@ -766,7 +766,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B17">
         <v>18</v>
@@ -786,12 +786,12 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>701</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>80</v>
@@ -831,12 +831,12 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B22">
         <v>538</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>243</v>
@@ -876,12 +876,12 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B25">
         <v>371</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B26">
         <v>195</v>
@@ -921,7 +921,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B27">
         <v>215</v>
@@ -941,12 +941,12 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B29">
         <v>395</v>
@@ -966,7 +966,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B30">
         <v>269</v>
@@ -986,7 +986,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B31">
         <v>113</v>

</xml_diff>